<commit_message>
Atualiza a planilha do repositório
</commit_message>
<xml_diff>
--- a/FII Sheet.xlsx
+++ b/FII Sheet.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educadventista-my.sharepoint.com/personal/rafael_garcia_educadventista_org/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="458" documentId="8_{F225B35B-8E70-4523-A8B1-573197FD46AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BF3B985-CE9E-422E-BBAB-8CE70D5755EF}"/>
+  <xr:revisionPtr revIDLastSave="585" documentId="8_{F225B35B-8E70-4523-A8B1-573197FD46AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35EE03A7-19E4-4987-8982-84A152F0C56E}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="3585" windowWidth="38700" windowHeight="15345" xr2:uid="{97DE1590-492C-4814-9651-8C0364570A6C}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{97DE1590-492C-4814-9651-8C0364570A6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha Auxiliar" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="aporte">Planilha1!$D$15</definedName>
-    <definedName name="qtde_anos">Planilha1!$D$16</definedName>
+    <definedName name="aporte">Planilha1!$D$6</definedName>
+    <definedName name="qtde_anos">Planilha1!$D$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
-  <si>
-    <t>Quanto investir por mês?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>Por quantos anos?</t>
   </si>
@@ -55,9 +52,6 @@
     <t>Dividendos mensais?</t>
   </si>
   <si>
-    <t>Investimento Mensal</t>
-  </si>
-  <si>
     <t>Quanto em 2 anos?</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Hotelarias</t>
   </si>
   <si>
-    <t>Valor a Investir</t>
-  </si>
-  <si>
     <t>Tipo de FII</t>
   </si>
   <si>
@@ -136,9 +127,6 @@
     <t>Sugerido (%)</t>
   </si>
   <si>
-    <t>Porcentagem a Investir</t>
-  </si>
-  <si>
     <t>Distribuição Sugerida por Perfil</t>
   </si>
   <si>
@@ -166,7 +154,16 @@
     <t>Diferença (%)</t>
   </si>
   <si>
-    <t>Planilha De Investimentos em Fundos Imobiliários</t>
+    <t>Simulação de Investimentos em Fundos Imobiliários</t>
+  </si>
+  <si>
+    <t>Valor a Investir Por Mês (R$)</t>
+  </si>
+  <si>
+    <t>Valor a Investir Por Mês (%)</t>
+  </si>
+  <si>
+    <t>Simulação</t>
   </si>
 </sst>
 </file>
@@ -176,19 +173,12 @@
   <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;R$&quot;\ #,##0;[Red]\-&quot;R$&quot;\ #,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="\+0.00%;\-0.00%;0.00%"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +245,12 @@
       <name val="Daytona"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -294,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -327,15 +323,6 @@
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thick">
         <color indexed="64"/>
       </top>
@@ -562,18 +549,54 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
       <right style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
-      <top/>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
       <bottom style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
       <right style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
@@ -589,187 +612,99 @@
       <left style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
       <bottom style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+      <right/>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
       </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+      <top style="thick">
+        <color theme="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+      <left style="thick">
+        <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -780,7 +715,7 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -790,10 +725,10 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -802,200 +737,200 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -1100,6 +1035,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1165,8 +1110,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{251C21B7-5D39-4A23-8018-16A8F3A80109}" name="Tabela4" displayName="Tabela4" ref="I24:K29" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="I24:K29" xr:uid="{251C21B7-5D39-4A23-8018-16A8F3A80109}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{251C21B7-5D39-4A23-8018-16A8F3A80109}" name="Tabela4" displayName="Tabela4" ref="F24:H29" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="F24:H29" xr:uid="{251C21B7-5D39-4A23-8018-16A8F3A80109}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{573554BA-E1A7-46B3-93B0-1395DCCF292F}" name="Nome" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{944B710A-3D75-43AA-BB62-FC93B6DFF3B1}" name="Tipo" dataDxfId="1"/>
@@ -1495,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572EB6BB-F1F4-40D0-82DA-F7B46AC3E394}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,32 +1450,34 @@
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="65" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
+    <row r="1" spans="1:14" s="35" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
     </row>
     <row r="2" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -1551,83 +1498,77 @@
     <row r="3" spans="1:14" ht="32.25" thickTop="1" x14ac:dyDescent="0.6">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="62"/>
+      <c r="C3" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="33"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
+      <c r="F3" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="12">
+      <c r="C4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="37">
         <v>1000</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="43" t="s">
-        <v>40</v>
+      <c r="F4" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="57" t="s">
+        <v>36</v>
       </c>
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="13">
+      <c r="C5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="38">
         <v>0.3</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="27">
-        <f>VLOOKUP($D$8&amp;"-"&amp;I5,'Planilha Auxiliar'!A1:D19,4,FALSE)</f>
+      <c r="F5" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="21">
+        <f>VLOOKUP($D$10&amp;"-"&amp;F5,'Planilha Auxiliar'!A1:D19,4,FALSE)</f>
         <v>0.5</v>
       </c>
-      <c r="K5" s="47">
-        <f t="shared" ref="K5:K10" si="0">$D$7*J5</f>
+      <c r="H5" s="29">
+        <f>$D$6*G5</f>
         <v>150</v>
       </c>
-      <c r="L5" s="27">
-        <f>SUMIF(Tabela4[Tipo], $I5, Tabela4[Valor]) / $D$7</f>
+      <c r="I5" s="21">
+        <f>SUMIF(Tabela4[Tipo], $F5, Tabela4[Valor]) /$D$6</f>
         <v>0</v>
       </c>
-      <c r="M5" s="48">
-        <f>L5-J5</f>
+      <c r="J5" s="59">
+        <f>I5-G5</f>
         <v>-0.5</v>
       </c>
       <c r="N5" s="2"/>
@@ -1635,33 +1576,31 @@
     <row r="6" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="14">
-        <v>6.0000000000000001E-3</v>
+      <c r="C6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="13">
+        <f>D4*D5</f>
+        <v>300</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="27">
-        <f>VLOOKUP($D$8&amp;"-"&amp;I6,'Planilha Auxiliar'!A2:D20,4,FALSE)</f>
+      <c r="F6" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="21">
+        <f>VLOOKUP($D$10&amp;"-"&amp;F6,'Planilha Auxiliar'!A2:D20,4,FALSE)</f>
         <v>0.3</v>
       </c>
-      <c r="K6" s="47">
-        <f t="shared" si="0"/>
+      <c r="H6" s="29">
+        <f t="shared" ref="H6:H10" si="0">$D$6*G6</f>
         <v>90</v>
       </c>
-      <c r="L6" s="27">
-        <f>SUMIF(Tabela4[Tipo], $I6, Tabela4[Valor]) / $D$7</f>
+      <c r="I6" s="21">
+        <f>SUMIF(Tabela4[Tipo], $F6, Tabela4[Valor]) /$D$6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="48">
-        <f t="shared" ref="M6:M10" si="1">L6-J6</f>
+      <c r="J6" s="59">
+        <f t="shared" ref="J6:J10" si="1">I6-G6</f>
         <v>-0.3</v>
       </c>
       <c r="N6" s="2"/>
@@ -1669,95 +1608,91 @@
     <row r="7" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="11" t="s">
-        <v>22</v>
+      <c r="C7" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="D7" s="15">
-        <f>D4*D5</f>
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="27">
-        <f>VLOOKUP($D$8&amp;"-"&amp;I7,'Planilha Auxiliar'!A3:D21,4,FALSE)</f>
+      <c r="F7" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="21">
+        <f>VLOOKUP($D$10&amp;"-"&amp;F7,'Planilha Auxiliar'!A3:D21,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="K7" s="47">
+      <c r="H7" s="29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="L7" s="27">
-        <f>SUMIF(Tabela4[Tipo], $I7, Tabela4[Valor]) / $D$7</f>
+      <c r="I7" s="21">
+        <f>SUMIF(Tabela4[Tipo], $F7, Tabela4[Valor]) /$D$6</f>
         <v>0</v>
       </c>
-      <c r="M7" s="48">
+      <c r="J7" s="59">
         <f t="shared" si="1"/>
         <v>-0.1</v>
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="22.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>14</v>
+      <c r="C8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="39">
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="27">
-        <f>VLOOKUP($D$8&amp;"-"&amp;I8,'Planilha Auxiliar'!A4:D22,4,FALSE)</f>
+      <c r="F8" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="21">
+        <f>VLOOKUP($D$10&amp;"-"&amp;F8,'Planilha Auxiliar'!A4:D22,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="K8" s="47">
+      <c r="H8" s="29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="L8" s="27">
-        <f>SUMIF(Tabela4[Tipo], $I8, Tabela4[Valor]) / $D$7</f>
+      <c r="I8" s="21">
+        <f>SUMIF(Tabela4[Tipo], $F8, Tabela4[Valor]) /$D$6</f>
         <v>0</v>
       </c>
-      <c r="M8" s="48">
+      <c r="J8" s="59">
         <f t="shared" si="1"/>
         <v>-0.1</v>
       </c>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="22.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
+      <c r="C9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1.0789999999999999E-2</v>
+      </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="27">
-        <f>VLOOKUP($D$8&amp;"-"&amp;I9,'Planilha Auxiliar'!A5:D23,4,FALSE)</f>
+      <c r="F9" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="21">
+        <f>VLOOKUP($D$10&amp;"-"&amp;F9,'Planilha Auxiliar'!A5:D23,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="47">
+      <c r="H9" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L9" s="27">
-        <f>SUMIF(Tabela4[Tipo], $I9, Tabela4[Valor]) / $D$7</f>
+      <c r="I9" s="21">
+        <f>SUMIF(Tabela4[Tipo], $F9, Tabela4[Valor]) /$D$6</f>
         <v>0</v>
       </c>
-      <c r="M9" s="48">
+      <c r="J9" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1766,38 +1701,37 @@
     <row r="10" spans="1:14" ht="22.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="50">
-        <f>VLOOKUP($D$8&amp;"-"&amp;I10,'Planilha Auxiliar'!A6:D24,4,FALSE)</f>
+      <c r="F10" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="61">
+        <f>VLOOKUP($D$10&amp;"-"&amp;F10,'Planilha Auxiliar'!A6:D24,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="51">
+      <c r="H10" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L10" s="50">
-        <f>SUMIF(Tabela4[Tipo], $I10, Tabela4[Valor]) / $D$7</f>
+      <c r="I10" s="61">
+        <f>SUMIF(Tabela4[Tipo], $F10, Tabela4[Valor]) /$D$6</f>
         <v>0</v>
       </c>
-      <c r="M10" s="52">
+      <c r="J10" s="63">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1844,21 +1778,23 @@
     <row r="14" spans="1:14" ht="32.25" thickTop="1" x14ac:dyDescent="0.6">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="60"/>
+      <c r="C14" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="31"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="63"/>
-      <c r="K14" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="F14" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1866,82 +1802,69 @@
     <row r="15" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="19">
-        <v>1260</v>
+      <c r="C15" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="17">
+        <f>FV(D9,D7*12,D6*-1)</f>
+        <v>8168.2881892935648</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15" s="28">
-        <f>FV($D$17,$B23*12,$D$15*-1)</f>
-        <v>34306.810395032975</v>
-      </c>
-      <c r="K15" s="29">
-        <f>J15*$D$6</f>
-        <v>205.84086237019787</v>
+      <c r="F15" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="24">
+        <f>FV($D$9,$B23*12,$D$6*-1)</f>
+        <v>8168.2881892935648</v>
+      </c>
+      <c r="H15" s="49">
+        <f>G15*$D$8</f>
+        <v>49.00972913576139</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="22.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="21">
-        <v>10</v>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="19">
+        <f>D15*D8</f>
+        <v>49.00972913576139</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="30">
-        <f>FV($D$17,$B24*12,$D$15*-1)</f>
-        <v>105558.91163809443</v>
-      </c>
-      <c r="K16" s="31">
-        <f>J16*$D$6</f>
-        <v>633.35346982856663</v>
+      <c r="F16" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="24">
+        <f>FV($D$9,$B24*12,$D$6*-1)</f>
+        <v>25133.074199546292</v>
+      </c>
+      <c r="H16" s="49">
+        <f>G16*$D$8</f>
+        <v>150.79844519727774</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" ht="22.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="22">
-        <v>1.0789999999999999E-2</v>
-      </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="30">
-        <f>FV($D$17,$B25*12,$D$15*-1)</f>
-        <v>306538.10778801696</v>
-      </c>
-      <c r="K17" s="31">
-        <f>J17*$D$6</f>
-        <v>1839.2286467281017</v>
+      <c r="F17" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="24">
+        <f>FV($D$9,$B25*12,$D$6*-1)</f>
+        <v>72985.263759051653</v>
+      </c>
+      <c r="H17" s="49">
+        <f>G17*$D$8</f>
+        <v>437.91158255430992</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1950,27 +1873,17 @@
     <row r="18" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="23">
-        <f>FV(D17,D16*12,D15*-1)</f>
-        <v>306538.10778801696</v>
-      </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="30">
-        <f>FV($D$17,$B26*12,$D$15*-1)</f>
-        <v>1417749.9841223215</v>
-      </c>
-      <c r="K18" s="31">
-        <f>J18*$D$6</f>
-        <v>8506.4999047339297</v>
+      <c r="F18" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="24">
+        <f>FV($D$9,$B26*12,$D$6*-1)</f>
+        <v>337559.52002912416</v>
+      </c>
+      <c r="H18" s="49">
+        <f>G18*$D$8</f>
+        <v>2025.357120174745</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1979,27 +1892,17 @@
     <row r="19" spans="1:14" ht="22.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="25">
-        <f>D18*D6</f>
-        <v>1839.2286467281017</v>
-      </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="32">
-        <f>FV($D$17,$B27*12,$D$15*-1)</f>
-        <v>5445933.7653059401</v>
-      </c>
-      <c r="K19" s="33">
-        <f>J19*$D$6</f>
-        <v>32675.602591835643</v>
+      <c r="F19" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="51">
+        <f>FV($D$9,$B27*12,$D$6*-1)</f>
+        <v>1296650.8965014142</v>
+      </c>
+      <c r="H19" s="52">
+        <f>G19*$D$8</f>
+        <v>7779.9053790084854</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -2041,19 +1944,19 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="31.5" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:14" ht="32.25" thickTop="1" x14ac:dyDescent="0.6">
       <c r="A23" s="2"/>
       <c r="B23" s="3">
         <v>2</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="54"/>
-      <c r="K23" s="55"/>
+      <c r="F23" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="65"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="44"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2063,17 +1966,14 @@
       <c r="B24" s="3">
         <v>5</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="K24" s="45" t="s">
-        <v>37</v>
+      <c r="F24" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -2084,12 +1984,9 @@
       <c r="B25" s="3">
         <v>10</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="36"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="23"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2099,12 +1996,9 @@
       <c r="B26" s="3">
         <v>20</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="37"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="25"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2114,12 +2008,9 @@
       <c r="B27" s="3">
         <v>30</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="37"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="25"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2130,33 +2021,27 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="37"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="25"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" ht="22.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="40"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="27"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2365,20 +2250,26 @@
       <c r="N42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F3:J3"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="I14:J14"/>
   </mergeCells>
+  <conditionalFormatting sqref="J5:J10">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>ABS(J5) &gt;10%</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{CFA5F8C6-F9AF-47B2-B2DF-2D88DE4C7A6C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10" xr:uid="{CFA5F8C6-F9AF-47B2-B2DF-2D88DE4C7A6C}">
       <formula1>"Conservador,Moderado,Agressivo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J25:J29" xr:uid="{C31B7CCC-0E25-445A-9A27-5FC04088694D}">
-      <formula1>$I$5:$I$10</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G25:G29" xr:uid="{C31B7CCC-0E25-445A-9A27-5FC04088694D}">
+      <formula1>$F$5:$F$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2407,16 +2298,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2425,10 +2316,10 @@
         <v>Conservador-Papel</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>0.5</v>
@@ -2440,10 +2331,10 @@
         <v>Conservador-Tijolo</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>0.3</v>
@@ -2455,10 +2346,10 @@
         <v>Conservador-Híbridos</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <v>0.1</v>
@@ -2471,10 +2362,10 @@
         <v>Conservador-FOFs</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1">
         <v>0.1</v>
@@ -2486,10 +2377,10 @@
         <v>Conservador-Desenvolvimento</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -2501,10 +2392,10 @@
         <v>Conservador-Hotelarias</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="8">
         <v>0</v>
@@ -2516,10 +2407,10 @@
         <v>Moderado-Papel</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1">
         <v>0.4</v>
@@ -2531,10 +2422,10 @@
         <v>Moderado-Tijolo</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1">
         <v>0.35</v>
@@ -2546,10 +2437,10 @@
         <v>Moderado-Híbridos</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
         <v>0.1</v>
@@ -2561,10 +2452,10 @@
         <v>Moderado-FOFs</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1">
         <v>0.05</v>
@@ -2576,10 +2467,10 @@
         <v>Moderado-Desenvolvimento</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
         <v>0.05</v>
@@ -2591,10 +2482,10 @@
         <v>Moderado-Hotelarias</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="8">
         <v>0.05</v>
@@ -2606,10 +2497,10 @@
         <v>Agressivo-Papel</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1">
         <v>0.3</v>
@@ -2621,10 +2512,10 @@
         <v>Agressivo-Tijolo</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1">
         <v>0.4</v>
@@ -2636,10 +2527,10 @@
         <v>Agressivo-Híbridos</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1">
         <v>0.05</v>
@@ -2651,10 +2542,10 @@
         <v>Agressivo-FOFs</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1">
         <v>0.1</v>
@@ -2666,10 +2557,10 @@
         <v>Agressivo-Desenvolvimento</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1">
         <v>0.1</v>
@@ -2681,10 +2572,10 @@
         <v>Agressivo-Hotelarias</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1">
         <v>0.05</v>

</xml_diff>